<commit_message>
Fixed Max function. Added numeric value support to CellInfo. Fixed a few bugs
</commit_message>
<xml_diff>
--- a/EPPlusTest/Workbooks/chainname.xlsx
+++ b/EPPlusTest/Workbooks/chainname.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17835"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17835" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="Name">Sheet1!$C$1</definedName>
@@ -342,7 +343,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -425,4 +426,74 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:XFD11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f>SUM(A1:A5)</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f>AVERAGE(A1:A5)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f>MAX(A1:A5)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <f>MIN(A1:A5)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <f>SUBTOTAL(6,A1:A5)</f>
+        <v>120</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>